<commit_message>
simulated PAA20, PAA25, PAA40, PAA45, PAA50 and compiled results
</commit_message>
<xml_diff>
--- a/PAA/results_MD.xlsx
+++ b/PAA/results_MD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="20unit" sheetId="2" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="40unit" sheetId="3" r:id="rId5"/>
     <sheet name="45unit" sheetId="7" r:id="rId6"/>
     <sheet name="50unit" sheetId="4" r:id="rId7"/>
+    <sheet name="summary" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="22">
   <si>
     <t>conformer</t>
   </si>
@@ -74,12 +75,27 @@
   </si>
   <si>
     <t>conf10</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Uncharged hydration</t>
+  </si>
+  <si>
+    <t>Charged</t>
+  </si>
+  <si>
+    <t>Difference</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0000E+00"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -109,10 +125,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,15 +434,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A8"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,28 +450,32 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>8991.1643627819994</v>
       </c>
-      <c r="D2" s="1">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1">
-        <f xml:space="preserve"> B2-D2</f>
-        <v>8990.1643627819994</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C2" s="1"/>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>60541.665058049999</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>A2+1</f>
         <v>1</v>
@@ -462,47 +483,50 @@
       <c r="B3" s="1">
         <v>8138.9970578769999</v>
       </c>
-      <c r="D3" s="1">
+      <c r="C3" s="1"/>
+      <c r="D3">
         <v>1</v>
       </c>
-      <c r="F3" s="1">
-        <f t="shared" ref="F3:F5" si="0" xml:space="preserve"> B3-D3</f>
-        <v>8137.9970578769999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E3" s="1">
+        <v>59887.489516349997</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f t="shared" ref="A4:A5" si="1">A3+1</f>
+        <f t="shared" ref="A4:A5" si="0">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>6827.0257726769996</v>
       </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1">
-        <f t="shared" si="0"/>
-        <v>6826.0257726769996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C4" s="1"/>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>62303.262523079997</v>
+      </c>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>7394.7008309960001</v>
       </c>
-      <c r="D5" s="1">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1">
-        <f t="shared" si="0"/>
-        <v>7393.7008309960001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C5" s="1"/>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1">
+        <v>65725.227655349998</v>
+      </c>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -510,16 +534,16 @@
         <f>AVERAGE(B2:B5)</f>
         <v>7837.9720060829995</v>
       </c>
-      <c r="D6" s="1">
-        <f>AVERAGE(D2:D5)</f>
-        <v>1</v>
-      </c>
-      <c r="F6" s="1">
-        <f>AVERAGE(F2:F5)</f>
-        <v>7836.9720060829995</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C6" s="1"/>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1">
+        <v>59617.148468519998</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -528,15 +552,13 @@
         <v>812.24539316289656</v>
       </c>
       <c r="D7">
-        <f>_xlfn.STDEV.P(D2:D5)</f>
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <f>_xlfn.STDEV.P(F2:F5)</f>
-        <v>812.24539316289656</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="E7" s="2">
+        <v>62247.911631870003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -545,12 +567,45 @@
         <v>10.362953485066265</v>
       </c>
       <c r="D8">
-        <f>D7/D6*100</f>
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <f>ABS(F7/F6*100)</f>
-        <v>10.364275801067526</v>
+        <v>6</v>
+      </c>
+      <c r="E8" s="2">
+        <v>57112.840461289998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9" s="2">
+        <v>63583.3892978</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1">
+        <f>AVERAGE(E2:E9)</f>
+        <v>61377.366826538746</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <f>_xlfn.STDEV.P(E2:E9)</f>
+        <v>2489.684861143628</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <f>E11/E10*100</f>
+        <v>4.0563565852862915</v>
       </c>
     </row>
   </sheetData>
@@ -560,109 +615,174 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2">
         <v>10801.971864020001</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>69529.430678150005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2">
         <v>15594.303937639999</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>70954.831248000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="2">
         <v>14424.73642974</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>70757.301643839994</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="2">
         <v>9814.0429821109992</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2">
+        <v>70576.321490600007</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="2">
         <v>11648.24923157</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6" s="2">
+        <v>77699.794937059996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="2">
         <v>14661.129507539999</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7" s="2">
+        <v>71342.686029460005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="2">
         <v>11359.55700257</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1">
+        <f>AVERAGE(E2:E7)</f>
+        <v>71810.061004518328</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="2">
         <v>13404.386412330001</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <f>_xlfn.STDEV.P(E2:E7)</f>
+        <v>2691.6696567102504</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <f>AVERAGE(B2:B9)</f>
         <v>12713.547170940124</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <f>E9/E8*100</f>
+        <v>3.7483182983800685</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <f>_xlfn.STDEV.P(B2:B9)</f>
+        <v>1953.4155284505189</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>5</v>
+      </c>
+      <c r="B12">
+        <f>B11/B10*100</f>
+        <v>15.364834866193133</v>
       </c>
     </row>
   </sheetData>
@@ -675,7 +795,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -933,15 +1053,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -949,122 +1072,189 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
-        <f>1</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>16101.66694064</v>
       </c>
-      <c r="D2" s="2">
+      <c r="C2" s="2"/>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
         <v>104314.65297919999</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>A2+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>18095.125933719999</v>
       </c>
-      <c r="D3" s="2">
+      <c r="C3" s="2"/>
+      <c r="D3">
+        <f>D2+1</f>
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
         <v>100552.12619559999</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <f t="shared" ref="A4:A9" si="0">A3+1</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>20389.14655569</v>
       </c>
-      <c r="D4" s="2">
+      <c r="C4" s="2"/>
+      <c r="D4">
+        <f t="shared" ref="D4:D8" si="1">D3+1</f>
+        <v>2</v>
+      </c>
+      <c r="E4" s="2">
         <v>102059.44919299999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>20389.14655569</v>
       </c>
-      <c r="D5" s="2">
+      <c r="C5" s="2"/>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E5" s="2">
         <v>116281.5899563</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>14993.37007425</v>
       </c>
-      <c r="D6" s="2">
+      <c r="C6" s="2"/>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E6" s="2">
         <v>107863.3160904</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>15417.036986679999</v>
       </c>
-      <c r="D7" s="2">
+      <c r="C7" s="2"/>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E7" s="2">
         <v>103205.3000393</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>16489.719352740001</v>
       </c>
-      <c r="D8" s="2">
+      <c r="C8" s="2"/>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="E8" s="2">
         <v>95477.733044649998</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>21819.674838989999</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C9" s="2"/>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="1">
+        <f>AVERAGE(E2:E8)</f>
+        <v>104250.59535692143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="2">
-        <f xml:space="preserve"> AVERAGE(B2:B9)</f>
+      <c r="B10" s="1">
+        <f>AVERAGE(B2:B9)</f>
         <v>17961.860904800003</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C10" s="1"/>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <f>_xlfn.STDEV.P(E2:E8)</f>
+        <v>6027.748177356606</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <f>_xlfn.STDEV.P(B2:B9)</f>
+        <v>2439.249579780877</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <f>E10/E9*100</f>
+        <v>5.7819796200870428</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>5</v>
+      </c>
+      <c r="B12">
+        <f>B11/B10*100</f>
+        <v>13.580160723374874</v>
       </c>
     </row>
   </sheetData>
@@ -1074,15 +1264,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1090,13 +1283,16 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>0</f>
         <v>0</v>
@@ -1104,8 +1300,15 @@
       <c r="B2" s="2">
         <v>19349.26875078</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>113776.3991403</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>A2+1</f>
         <v>1</v>
@@ -1113,8 +1316,15 @@
       <c r="B3" s="2">
         <v>23892.04830572</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <f>D2+1</f>
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>113695.5765982</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <f t="shared" ref="A4:A7" si="0">A3+1</f>
         <v>2</v>
@@ -1122,8 +1332,15 @@
       <c r="B4" s="2">
         <v>19548.380330920001</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <f t="shared" ref="D4:D7" si="1">D3+1</f>
+        <v>2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>116178.2059167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1131,8 +1348,15 @@
       <c r="B5" s="2">
         <v>20608.84511278</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E5" s="2">
+        <v>107511.2696208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1140,8 +1364,15 @@
       <c r="B6" s="2">
         <v>21005.408782999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E6" s="2">
+        <v>114912.92748699999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1149,24 +1380,60 @@
       <c r="B7" s="2">
         <v>24160.360380189999</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E7" s="2">
+        <v>109040.099466</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="2">
-        <f xml:space="preserve"> AVERAGE(B2:B7)</f>
+      <c r="B8" s="1">
+        <f>AVERAGE(B2:B7)</f>
         <v>21427.385277231668</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1">
+        <f>AVERAGE(E2:E7)</f>
+        <v>112519.07970483333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <f>_xlfn.STDEV.P(B2:B7)</f>
+        <v>1925.314554632015</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <f>_xlfn.STDEV.P(E2:E7)</f>
+        <v>3142.8801621388711</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
+      </c>
+      <c r="B10">
+        <f>B9/B8*100</f>
+        <v>8.9852986247361564</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <f>E9/E8*100</f>
+        <v>2.7931975362609252</v>
       </c>
     </row>
   </sheetData>
@@ -1176,15 +1443,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1192,21 +1462,30 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>22635.752544480001</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>133335.0567013</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>A2+1</f>
         <v>1</v>
@@ -1214,8 +1493,15 @@
       <c r="B3" s="2">
         <v>17986.163607350001</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <f>D2+1</f>
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>127129.804641</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <f t="shared" ref="A4:A9" si="0">A3+1</f>
         <v>2</v>
@@ -1223,8 +1509,15 @@
       <c r="B4" s="2">
         <v>19410.541362420001</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <f t="shared" ref="D4:D7" si="1">D3+1</f>
+        <v>2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>125186.6613239</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1232,8 +1525,15 @@
       <c r="B5" s="2">
         <v>21255.18521711</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E5" s="2">
+        <v>131551.79052929999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1241,8 +1541,15 @@
       <c r="B6" s="2">
         <v>19355.557858249998</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E6" s="2">
+        <v>121384.32513500001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1250,8 +1557,15 @@
       <c r="B7" s="2">
         <v>19854.659100559998</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E7" s="2">
+        <v>128039.0239764</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1259,8 +1573,15 @@
       <c r="B8" s="2">
         <v>22897.162346559999</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1">
+        <f>AVERAGE(E2:E7)</f>
+        <v>127771.11038448334</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1268,8 +1589,15 @@
       <c r="B9" s="2">
         <v>23267.346453300001</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <f>_xlfn.STDEV.P(E2:E7)</f>
+        <v>3941.3300312829028</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>A9+1</f>
         <v>8</v>
@@ -1277,24 +1605,39 @@
       <c r="B10" s="2">
         <v>20163.301284130001</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <f>E9/E8*100</f>
+        <v>3.0846801122905028</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="2">
-        <f xml:space="preserve"> AVERAGE(B2:B10)</f>
+      <c r="B11" s="1">
+        <f>AVERAGE(B2:B10)</f>
         <v>20758.407752684448</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <f>_xlfn.STDEV.P(B2:B10)</f>
+        <v>1741.0481677396292</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>5</v>
+      </c>
+      <c r="B13">
+        <f>B12/B11*100</f>
+        <v>8.3871951475395772</v>
       </c>
     </row>
   </sheetData>
@@ -1304,93 +1647,147 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2">
         <v>24585.840178679999</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3">
+        <v>138099.20416309999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2">
         <v>27343.492583849998</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3">
+        <v>142014.7865775</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="2">
         <v>28796.000521459999</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3">
+        <v>137716.15445629999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="2">
         <v>26519.5327339</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3">
+        <v>141544.4420372</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="2">
         <v>26640.543960840001</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="3">
+        <v>148485.4252385</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="2">
         <v>25456.900521390002</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1">
+        <f>AVERAGE(E2:E6)</f>
+        <v>141572.00249451998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="2">
         <v>22927.854093739999</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <f>_xlfn.STDEV.P(E2:E6)</f>
+        <v>3870.9203997108175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="2">
         <v>23602.932673930001</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <f>E8/E7*100</f>
+        <v>2.7342414683020779</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1398,7 +1795,7 @@
         <v>21452.69447893</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1406,7 +1803,7 @@
         <v>26384.34232127</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1414,23 +1811,189 @@
         <v>22942.05577843</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="2">
-        <f xml:space="preserve"> AVERAGE(B2:B12)</f>
+      <c r="B13" s="1">
+        <f>AVERAGE(B2:B12)</f>
         <v>25150.199076947276</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <f>_xlfn.STDEV.P(B2:B12)</f>
+        <v>2132.3177963782164</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>5</v>
+      </c>
+      <c r="B15">
+        <f>B14/B13*100</f>
+        <v>8.4783336698622929</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1">
+        <f>'20unit'!B6</f>
+        <v>7837.9720060829995</v>
+      </c>
+      <c r="C2" s="1">
+        <f>'20unit'!E10</f>
+        <v>61377.366826538746</v>
+      </c>
+      <c r="D2" s="1">
+        <f xml:space="preserve"> C2-B2</f>
+        <v>53539.394820455746</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f>A2+5</f>
+        <v>25</v>
+      </c>
+      <c r="B3" s="1">
+        <f>'25unit'!B10</f>
+        <v>12713.547170940124</v>
+      </c>
+      <c r="C3" s="1">
+        <f>'25unit'!E8</f>
+        <v>71810.061004518328</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D8" si="0" xml:space="preserve"> C3-B3</f>
+        <v>59096.513833578203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f t="shared" ref="A4:A8" si="1">A3+5</f>
+        <v>30</v>
+      </c>
+      <c r="B4" s="1">
+        <f>'30unit'!B13</f>
+        <v>14990.145237377274</v>
+      </c>
+      <c r="C4" s="1">
+        <f>'30unit'!D13</f>
+        <v>100054.14899207363</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>85064.003754696358</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="B5" s="1">
+        <f>'35unit'!B10</f>
+        <v>17961.860904800003</v>
+      </c>
+      <c r="C5" s="1">
+        <f>'35unit'!E9</f>
+        <v>104250.59535692143</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>86288.734452121425</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="B6" s="1">
+        <f>'40unit'!B8</f>
+        <v>21427.385277231668</v>
+      </c>
+      <c r="C6" s="1">
+        <f>'40unit'!E8</f>
+        <v>112519.07970483333</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>91091.694427601673</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="B7" s="1">
+        <f>'45unit'!B11</f>
+        <v>20758.407752684448</v>
+      </c>
+      <c r="C7" s="1">
+        <f>'45unit'!E8</f>
+        <v>127771.11038448334</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>107012.70263179889</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="B8" s="1">
+        <f>'50unit'!B13</f>
+        <v>25150.199076947276</v>
+      </c>
+      <c r="C8" s="1">
+        <f>'50unit'!E7</f>
+        <v>141572.00249451998</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>116421.80341757271</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
compared solvation energy results
</commit_message>
<xml_diff>
--- a/PAA/results_MD.xlsx
+++ b/PAA/results_MD.xlsx
@@ -94,7 +94,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.0000E+00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -129,7 +129,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1848,7 +1848,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>